<commit_message>
Changed mapping of cha2sxrg from "InitialCharge" to "FinalCharge"
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/vermont/Vermont_Disposition_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/vermont/Vermont_Disposition_Mapping.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="655">
   <si>
     <t>BRISTOL P.D.</t>
   </si>
@@ -2010,6 +2010,9 @@
   </si>
   <si>
     <t>Need definition clarification ?</t>
+  </si>
+  <si>
+    <t>/exchange:DispositionReport/nc:Case/j:CaseAugmentation/j:CaseCharge/ext:ChargeAugmentation/ext:FinalCharge/ext:ChargeAugmentation/ext:SexRegistryChargeIndicator</t>
   </si>
 </sst>
 </file>
@@ -2206,16 +2209,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2536,8 +2539,8 @@
   <dimension ref="A1:E139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E114" sqref="E114"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -2568,7 +2571,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>581</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -2582,7 +2585,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="12" t="s">
         <v>582</v>
       </c>
@@ -3144,10 +3147,10 @@
       <c r="B44" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="C44" s="21" t="s">
         <v>574</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="21" t="s">
         <v>603</v>
       </c>
     </row>
@@ -3158,8 +3161,8 @@
       <c r="B45" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
     </row>
     <row r="46" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
@@ -3168,8 +3171,8 @@
       <c r="B46" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
     </row>
     <row r="47" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
@@ -3315,10 +3318,10 @@
       <c r="B57" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="C57" s="21" t="s">
         <v>574</v>
       </c>
-      <c r="D57" s="19" t="s">
+      <c r="D57" s="21" t="s">
         <v>604</v>
       </c>
     </row>
@@ -3329,8 +3332,8 @@
       <c r="B58" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
     </row>
     <row r="59" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
@@ -3339,8 +3342,8 @@
       <c r="B59" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
     </row>
     <row r="60" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
@@ -3363,10 +3366,10 @@
       <c r="B61" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="C61" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="D61" s="19" t="s">
+      <c r="D61" s="21" t="s">
         <v>605</v>
       </c>
     </row>
@@ -3377,8 +3380,8 @@
       <c r="B62" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
     </row>
     <row r="63" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
@@ -3387,8 +3390,8 @@
       <c r="B63" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
     </row>
     <row r="64" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
@@ -3758,10 +3761,10 @@
       <c r="B91" s="6" t="s">
         <v>433</v>
       </c>
-      <c r="C91" s="19" t="s">
+      <c r="C91" s="21" t="s">
         <v>574</v>
       </c>
-      <c r="D91" s="19" t="s">
+      <c r="D91" s="21" t="s">
         <v>610</v>
       </c>
     </row>
@@ -3772,8 +3775,8 @@
       <c r="B92" s="6" t="s">
         <v>434</v>
       </c>
-      <c r="C92" s="20"/>
-      <c r="D92" s="20"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="22"/>
     </row>
     <row r="93" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
@@ -3782,8 +3785,8 @@
       <c r="B93" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="C93" s="20"/>
-      <c r="D93" s="20"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="22"/>
     </row>
     <row r="94" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="18" t="s">
@@ -3903,7 +3906,7 @@
         <v>503</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>561</v>
+        <v>654</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Merging from master to analytical-data-store-branch.  Merge was performed and followed by a clean build.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/vermont/Vermont_Disposition_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/vermont/Vermont_Disposition_Mapping.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="655">
   <si>
     <t>BRISTOL P.D.</t>
   </si>
@@ -2010,6 +2010,9 @@
   </si>
   <si>
     <t>Need definition clarification ?</t>
+  </si>
+  <si>
+    <t>/exchange:DispositionReport/nc:Case/j:CaseAugmentation/j:CaseCharge/ext:ChargeAugmentation/ext:FinalCharge/ext:ChargeAugmentation/ext:SexRegistryChargeIndicator</t>
   </si>
 </sst>
 </file>
@@ -2206,16 +2209,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2536,8 +2539,8 @@
   <dimension ref="A1:E139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E114" sqref="E114"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -2568,7 +2571,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>581</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -2582,7 +2585,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="12" t="s">
         <v>582</v>
       </c>
@@ -3144,10 +3147,10 @@
       <c r="B44" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="C44" s="21" t="s">
         <v>574</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="21" t="s">
         <v>603</v>
       </c>
     </row>
@@ -3158,8 +3161,8 @@
       <c r="B45" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
     </row>
     <row r="46" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
@@ -3168,8 +3171,8 @@
       <c r="B46" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
     </row>
     <row r="47" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
@@ -3315,10 +3318,10 @@
       <c r="B57" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="C57" s="21" t="s">
         <v>574</v>
       </c>
-      <c r="D57" s="19" t="s">
+      <c r="D57" s="21" t="s">
         <v>604</v>
       </c>
     </row>
@@ -3329,8 +3332,8 @@
       <c r="B58" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
     </row>
     <row r="59" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
@@ -3339,8 +3342,8 @@
       <c r="B59" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
     </row>
     <row r="60" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
@@ -3363,10 +3366,10 @@
       <c r="B61" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="C61" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="D61" s="19" t="s">
+      <c r="D61" s="21" t="s">
         <v>605</v>
       </c>
     </row>
@@ -3377,8 +3380,8 @@
       <c r="B62" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
     </row>
     <row r="63" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
@@ -3387,8 +3390,8 @@
       <c r="B63" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
     </row>
     <row r="64" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
@@ -3758,10 +3761,10 @@
       <c r="B91" s="6" t="s">
         <v>433</v>
       </c>
-      <c r="C91" s="19" t="s">
+      <c r="C91" s="21" t="s">
         <v>574</v>
       </c>
-      <c r="D91" s="19" t="s">
+      <c r="D91" s="21" t="s">
         <v>610</v>
       </c>
     </row>
@@ -3772,8 +3775,8 @@
       <c r="B92" s="6" t="s">
         <v>434</v>
       </c>
-      <c r="C92" s="20"/>
-      <c r="D92" s="20"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="22"/>
     </row>
     <row r="93" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
@@ -3782,8 +3785,8 @@
       <c r="B93" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="C93" s="20"/>
-      <c r="D93" s="20"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="22"/>
     </row>
     <row r="94" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="18" t="s">
@@ -3903,7 +3906,7 @@
         <v>503</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>561</v>
+        <v>654</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added "disp-ext:IsProbationViolationOnOldCharge" element for Vermont
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/vermont/Vermont_Disposition_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/vermont/Vermont_Disposition_Mapping.xlsx
@@ -36,7 +36,7 @@
     <sheet name="Sheet23" sheetId="29" r:id="rId27"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$A$1:$D$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$A$1:$D$124</definedName>
   </definedNames>
   <calcPr calcId="140001"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="658">
   <si>
     <t>BRISTOL P.D.</t>
   </si>
@@ -2013,13 +2013,22 @@
   </si>
   <si>
     <t>/exchange:DispositionReport/nc:Case/j:CaseAugmentation/j:CaseCharge/ext:ChargeAugmentation/ext:FinalCharge/ext:ChargeAugmentation/ext:SexRegistryChargeIndicator</t>
+  </si>
+  <si>
+    <t>True if charge is a probation violation, false otherwise.</t>
+  </si>
+  <si>
+    <t>NAME?</t>
+  </si>
+  <si>
+    <t>/disp-doc:DispositionReport/nc:Case/j:CaseAugmentation/j:CaseCharge/disp-ext:ChargeAugmentation/disp-ext:InitialCharge/disp-ext:ChargeAugmentation/disp-ext:IsProbationViolationOnOldCharge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2106,6 +2115,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2153,7 +2168,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2209,6 +2224,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2219,6 +2237,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2536,11 +2557,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E102" sqref="E102"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -2571,7 +2592,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>581</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -2585,7 +2606,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="12" t="s">
         <v>582</v>
       </c>
@@ -3147,10 +3168,10 @@
       <c r="B44" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="C44" s="22" t="s">
         <v>574</v>
       </c>
-      <c r="D44" s="21" t="s">
+      <c r="D44" s="22" t="s">
         <v>603</v>
       </c>
     </row>
@@ -3161,8 +3182,8 @@
       <c r="B45" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
     </row>
     <row r="46" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
@@ -3171,8 +3192,8 @@
       <c r="B46" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
     </row>
     <row r="47" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
@@ -3318,10 +3339,10 @@
       <c r="B57" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="22" t="s">
         <v>574</v>
       </c>
-      <c r="D57" s="21" t="s">
+      <c r="D57" s="22" t="s">
         <v>604</v>
       </c>
     </row>
@@ -3332,8 +3353,8 @@
       <c r="B58" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
     </row>
     <row r="59" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
@@ -3342,8 +3363,8 @@
       <c r="B59" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
     </row>
     <row r="60" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
@@ -3366,10 +3387,10 @@
       <c r="B61" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="C61" s="21" t="s">
+      <c r="C61" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="D61" s="21" t="s">
+      <c r="D61" s="22" t="s">
         <v>605</v>
       </c>
     </row>
@@ -3380,8 +3401,8 @@
       <c r="B62" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="C62" s="22"/>
-      <c r="D62" s="22"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
     </row>
     <row r="63" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
@@ -3390,8 +3411,8 @@
       <c r="B63" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="C63" s="22"/>
-      <c r="D63" s="22"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
     </row>
     <row r="64" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
@@ -3543,790 +3564,804 @@
         <v>593</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
+    <row r="75" spans="1:5" s="19" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="24" t="s">
+        <v>656</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>503</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B76" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="C75" s="12" t="s">
+      <c r="C76" s="12" t="s">
         <v>567</v>
       </c>
-      <c r="D75" s="12" t="s">
+      <c r="D76" s="12" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A76" s="8" t="s">
+    <row r="77" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="B77" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="C76" s="12" t="s">
+      <c r="C77" s="12" t="s">
         <v>503</v>
       </c>
-      <c r="D76" s="16" t="s">
+      <c r="D77" s="16" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="14" t="s">
+    <row r="78" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B78" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="E77" s="4" t="s">
+      <c r="E78" s="4" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="78" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
+    <row r="79" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B79" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="C78" s="12" t="s">
+      <c r="C79" s="12" t="s">
         <v>567</v>
       </c>
-      <c r="D78" s="12" t="s">
+      <c r="D79" s="12" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="14" t="s">
+    <row r="80" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B80" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="D79" s="11"/>
-      <c r="E79" s="4" t="s">
+      <c r="D80" s="11"/>
+      <c r="E80" s="4" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="80" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="8" t="s">
+    <row r="81" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B81" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="C80" s="12" t="s">
+      <c r="C81" s="12" t="s">
         <v>567</v>
       </c>
-      <c r="D80" s="12" t="s">
+      <c r="D81" s="12" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="81" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A81" s="8" t="s">
+    <row r="82" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="B82" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="C81" s="12" t="s">
+      <c r="C82" s="12" t="s">
         <v>503</v>
       </c>
-      <c r="D81" s="12" t="s">
+      <c r="D82" s="12" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="82" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="s">
+    <row r="83" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B83" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="D82" s="11"/>
-      <c r="E82" s="4" t="s">
+      <c r="D83" s="11"/>
+      <c r="E83" s="4" t="s">
         <v>515</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A83" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>504</v>
-      </c>
-      <c r="C83" s="12" t="s">
-        <v>503</v>
-      </c>
-      <c r="D83" s="13" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="D84" s="13" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A85" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="B84" s="6" t="s">
+      <c r="B85" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="C84" s="12" t="s">
+      <c r="C85" s="12" t="s">
         <v>571</v>
       </c>
-      <c r="D84" s="13" t="s">
+      <c r="D85" s="13" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="8" t="s">
+    <row r="86" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="B86" s="12" t="s">
         <v>490</v>
       </c>
-      <c r="C85" s="12" t="s">
+      <c r="C86" s="12" t="s">
         <v>569</v>
       </c>
-      <c r="D85" s="12" t="s">
+      <c r="D86" s="12" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="18" t="s">
+    <row r="87" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="B86" s="6" t="s">
+      <c r="B87" s="6" t="s">
         <v>505</v>
       </c>
-      <c r="E86" s="12" t="s">
+      <c r="E87" s="12" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
+    <row r="88" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="C87" s="12" t="s">
+      <c r="C88" s="12" t="s">
         <v>568</v>
       </c>
-      <c r="D87" s="13" t="s">
+      <c r="D88" s="13" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A88" s="8" t="s">
+    <row r="89" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A89" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="B89" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="C88" s="12" t="s">
+      <c r="C89" s="12" t="s">
         <v>573</v>
       </c>
-      <c r="D88" s="13" t="s">
+      <c r="D89" s="13" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A89" s="8" t="s">
+    <row r="90" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B90" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="C89" s="12" t="s">
+      <c r="C90" s="12" t="s">
         <v>567</v>
       </c>
-      <c r="D89" s="13" t="s">
+      <c r="D90" s="13" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
+    <row r="91" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A91" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B91" s="6" t="s">
         <v>432</v>
       </c>
-      <c r="C90" s="12" t="s">
+      <c r="C91" s="12" t="s">
         <v>573</v>
       </c>
-      <c r="D90" s="12" t="s">
+      <c r="D91" s="12" t="s">
         <v>611</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="C91" s="21" t="s">
-        <v>574</v>
-      </c>
-      <c r="D91" s="21" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>434</v>
-      </c>
-      <c r="C92" s="22"/>
-      <c r="D92" s="22"/>
+        <v>433</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>574</v>
+      </c>
+      <c r="D92" s="22" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="93" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="C93" s="23"/>
+      <c r="D93" s="23"/>
+    </row>
+    <row r="94" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="B94" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="C93" s="22"/>
-      <c r="D93" s="22"/>
-    </row>
-    <row r="94" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="18" t="s">
+      <c r="C94" s="23"/>
+      <c r="D94" s="23"/>
+    </row>
+    <row r="95" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="B94" s="6" t="s">
+      <c r="B95" s="6" t="s">
         <v>436</v>
       </c>
-      <c r="E94" s="12" t="s">
+      <c r="E95" s="12" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="14" t="s">
+    <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="B95" s="7" t="s">
+      <c r="B96" s="7" t="s">
         <v>436</v>
       </c>
-      <c r="D95" s="9"/>
-      <c r="E95" s="4" t="s">
+      <c r="D96" s="9"/>
+      <c r="E96" s="4" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A96" s="8" t="s">
+    <row r="97" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A97" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="B96" s="6" t="s">
+      <c r="B97" s="6" t="s">
         <v>437</v>
       </c>
-      <c r="C96" s="12" t="s">
+      <c r="C97" s="12" t="s">
         <v>569</v>
       </c>
-      <c r="D96" s="13" t="s">
+      <c r="D97" s="13" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="8" t="s">
+    <row r="98" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B97" s="6" t="s">
+      <c r="B98" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="C97" s="12" t="s">
+      <c r="C98" s="12" t="s">
         <v>567</v>
       </c>
-      <c r="D97" s="12" t="s">
+      <c r="D98" s="12" t="s">
         <v>566</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A98" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B98" s="12" t="s">
-        <v>491</v>
-      </c>
-      <c r="C98" s="12" t="s">
-        <v>573</v>
-      </c>
-      <c r="D98" s="13" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C99" s="12" t="s">
         <v>573</v>
       </c>
       <c r="D99" s="13" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A100" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B100" s="12" t="s">
+        <v>492</v>
+      </c>
+      <c r="C100" s="12" t="s">
+        <v>573</v>
+      </c>
+      <c r="D100" s="13" t="s">
         <v>609</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>448</v>
-      </c>
-      <c r="C100" s="12" t="s">
-        <v>571</v>
-      </c>
-      <c r="D100" s="13" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C101" s="12" t="s">
         <v>571</v>
       </c>
-      <c r="D101" s="12" t="s">
-        <v>560</v>
+      <c r="D101" s="13" t="s">
+        <v>620</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>501</v>
+        <v>449</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>503</v>
+        <v>571</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>654</v>
+        <v>560</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="C103" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A104" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="B103" s="6" t="s">
+      <c r="B104" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="C103" s="12" t="s">
+      <c r="C104" s="12" t="s">
         <v>575</v>
       </c>
-      <c r="D103" s="12" t="s">
+      <c r="D104" s="12" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="14" t="s">
+    <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="B104" s="7" t="s">
+      <c r="B105" s="7" t="s">
         <v>451</v>
       </c>
-      <c r="D104" s="11"/>
-      <c r="E104" s="4" t="s">
+      <c r="D105" s="11"/>
+      <c r="E105" s="4" t="s">
         <v>481</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A105" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>452</v>
-      </c>
-      <c r="C105" s="12" t="s">
-        <v>571</v>
-      </c>
-      <c r="D105" s="12" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="106" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C106" s="12" t="s">
         <v>571</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="107" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C107" s="12" t="s">
         <v>571</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="108" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="C108" s="12" t="s">
+        <v>571</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A109" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="B108" s="6" t="s">
+      <c r="B109" s="6" t="s">
         <v>592</v>
       </c>
-      <c r="C108" s="12" t="s">
+      <c r="C109" s="12" t="s">
         <v>503</v>
       </c>
-      <c r="D108" s="13" t="s">
+      <c r="D109" s="13" t="s">
         <v>561</v>
       </c>
-      <c r="E108" s="12" t="s">
+      <c r="E109" s="12" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
+    <row r="110" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="B109" s="12" t="s">
+      <c r="B110" s="12" t="s">
         <v>483</v>
       </c>
-      <c r="C109" s="12" t="s">
+      <c r="C110" s="12" t="s">
         <v>569</v>
       </c>
-      <c r="D109" s="12" t="s">
+      <c r="D110" s="12" t="s">
         <v>562</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A110" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>506</v>
-      </c>
-      <c r="C110" s="12" t="s">
-        <v>567</v>
-      </c>
-      <c r="D110" s="12" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="111" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="B111" s="12" t="s">
-        <v>493</v>
+        <v>219</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>506</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>569</v>
-      </c>
-      <c r="D111" s="13" t="s">
-        <v>616</v>
+        <v>567</v>
+      </c>
+      <c r="D111" s="12" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="112" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>469</v>
+        <v>220</v>
+      </c>
+      <c r="B112" s="12" t="s">
+        <v>493</v>
       </c>
       <c r="C112" s="12" t="s">
         <v>569</v>
       </c>
-      <c r="D112" s="12" t="s">
-        <v>564</v>
-      </c>
-      <c r="E112" s="12" t="s">
-        <v>579</v>
+      <c r="D112" s="13" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="113" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>621</v>
+        <v>469</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>567</v>
-      </c>
-      <c r="D113" s="16" t="s">
-        <v>622</v>
+        <v>569</v>
+      </c>
+      <c r="D113" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="E113" s="12" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="114" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>621</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>503</v>
-      </c>
-      <c r="D114" s="12" t="s">
-        <v>539</v>
-      </c>
-      <c r="E114" s="12" t="s">
-        <v>580</v>
+        <v>567</v>
+      </c>
+      <c r="D114" s="16" t="s">
+        <v>622</v>
       </c>
     </row>
     <row r="115" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="B115" s="12" t="s">
-        <v>494</v>
+        <v>223</v>
       </c>
       <c r="C115" s="12" t="s">
         <v>503</v>
       </c>
       <c r="D115" s="12" t="s">
+        <v>539</v>
+      </c>
+      <c r="E115" s="12" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A116" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B116" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="C116" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="D116" s="12" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A116" s="8" t="s">
+    <row r="117" spans="1:5" s="12" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A117" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="B116" s="12" t="s">
+      <c r="B117" s="12" t="s">
         <v>495</v>
       </c>
-      <c r="C116" s="12" t="s">
+      <c r="C117" s="12" t="s">
         <v>574</v>
       </c>
-      <c r="D116" s="12" t="s">
+      <c r="D117" s="12" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="14" t="s">
+    <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="D117" s="11"/>
-    </row>
-    <row r="118" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A118" s="8" t="s">
+      <c r="D118" s="11"/>
+    </row>
+    <row r="119" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A119" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="B118" s="12" t="s">
+      <c r="B119" s="12" t="s">
         <v>497</v>
       </c>
-      <c r="C118" s="12" t="s">
+      <c r="C119" s="12" t="s">
         <v>573</v>
       </c>
-      <c r="D118" s="12" t="s">
+      <c r="D119" s="12" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>498</v>
-      </c>
-      <c r="D119" s="11"/>
     </row>
     <row r="120" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="D120" s="11"/>
+    </row>
+    <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="B120" s="7" t="s">
+      <c r="B121" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="D120" s="11"/>
-    </row>
-    <row r="121" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A121" s="8" t="s">
+      <c r="D121" s="11"/>
+    </row>
+    <row r="122" spans="1:5" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A122" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="B121" s="12" t="s">
+      <c r="B122" s="12" t="s">
         <v>476</v>
       </c>
-      <c r="C121" s="12" t="s">
+      <c r="C122" s="12" t="s">
         <v>571</v>
       </c>
-      <c r="D121" s="12" t="s">
+      <c r="D122" s="12" t="s">
         <v>529</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="B122" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="C122" s="12" t="s">
-        <v>575</v>
-      </c>
-      <c r="D122" s="13" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="123" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="C123" s="12" t="s">
+        <v>575</v>
+      </c>
+      <c r="D123" s="13" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="B123" s="12" t="s">
+      <c r="B124" s="12" t="s">
         <v>502</v>
       </c>
-      <c r="C123" s="12" t="s">
+      <c r="C124" s="12" t="s">
         <v>577</v>
       </c>
-      <c r="D123" s="13" t="s">
+      <c r="D124" s="13" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="8"/>
-    </row>
     <row r="125" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="8" t="s">
+      <c r="A125" s="8"/>
+    </row>
+    <row r="126" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="8" t="s">
         <v>626</v>
       </c>
-      <c r="C125" s="12" t="s">
+      <c r="C126" s="12" t="s">
         <v>637</v>
       </c>
-      <c r="D125" s="16" t="s">
+      <c r="D126" s="16" t="s">
         <v>625</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D126" s="16" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D127" s="16" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="8" t="s">
         <v>627</v>
       </c>
-      <c r="D127" s="16" t="s">
+      <c r="D128" s="16" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="8"/>
-    </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="8" t="s">
-        <v>630</v>
-      </c>
-      <c r="C129" s="16" t="s">
-        <v>637</v>
-      </c>
-      <c r="D129" s="16" t="s">
-        <v>633</v>
-      </c>
+      <c r="A129" s="8"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
-        <v>631</v>
+        <v>630</v>
+      </c>
+      <c r="C130" s="16" t="s">
+        <v>637</v>
       </c>
       <c r="D130" s="16" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
+        <v>631</v>
+      </c>
+      <c r="D131" s="16" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="8" t="s">
         <v>632</v>
       </c>
-      <c r="D131" s="16" t="s">
+      <c r="D132" s="16" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="8"/>
-    </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="8" t="s">
-        <v>636</v>
-      </c>
-      <c r="C133" s="16" t="s">
-        <v>637</v>
-      </c>
-      <c r="D133" s="16" t="s">
-        <v>638</v>
-      </c>
+      <c r="A133" s="8"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
-        <v>122</v>
+        <v>636</v>
+      </c>
+      <c r="C134" s="16" t="s">
+        <v>637</v>
       </c>
       <c r="D134" s="16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D135" s="16" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="8" t="s">
         <v>640</v>
       </c>
-      <c r="D135" s="16" t="s">
+      <c r="D136" s="16" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="8"/>
-    </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="8" t="s">
-        <v>642</v>
-      </c>
-      <c r="C137" s="16" t="s">
-        <v>637</v>
-      </c>
-      <c r="D137" s="16" t="s">
-        <v>643</v>
-      </c>
+      <c r="A137" s="8"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
-        <v>632</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>647</v>
+        <v>642</v>
+      </c>
+      <c r="C138" s="16" t="s">
+        <v>637</v>
       </c>
       <c r="D138" s="16" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
+        <v>632</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="D139" s="16" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="8" t="s">
         <v>644</v>
       </c>
-      <c r="D139" s="16" t="s">
+      <c r="D140" s="16" t="s">
         <v>646</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D123"/>
+  <autoFilter ref="A1:D124"/>
   <mergeCells count="9">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="D61:D63"/>
     <mergeCell ref="D57:D59"/>
-    <mergeCell ref="D91:D93"/>
+    <mergeCell ref="D92:D94"/>
     <mergeCell ref="D44:D46"/>
     <mergeCell ref="C44:C46"/>
     <mergeCell ref="C57:C59"/>
     <mergeCell ref="C61:C63"/>
-    <mergeCell ref="C91:C93"/>
+    <mergeCell ref="C92:C94"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>